<commit_message>
Coordinates of phone and qwerty layouts
</commit_message>
<xml_diff>
--- a/layout/Coordinates.xlsx
+++ b/layout/Coordinates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>X</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Inner Radius</t>
   </si>
   <si>
-    <t>Circles</t>
-  </si>
-  <si>
     <t>Double Ring</t>
   </si>
   <si>
@@ -136,6 +133,45 @@
   </si>
   <si>
     <t>11*8.5</t>
+  </si>
+  <si>
+    <t>Square Size</t>
+  </si>
+  <si>
+    <t>0.8 * 0.8</t>
+  </si>
+  <si>
+    <t>2.1 * 2.1</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>GHI</t>
+  </si>
+  <si>
+    <t>JKL</t>
+  </si>
+  <si>
+    <t>MNO</t>
+  </si>
+  <si>
+    <t>PQRS</t>
+  </si>
+  <si>
+    <t>TUV</t>
+  </si>
+  <si>
+    <t>WXYZ</t>
+  </si>
+  <si>
+    <t>Group</t>
   </si>
 </sst>
 </file>
@@ -317,7 +353,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -340,12 +376,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
@@ -365,16 +395,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -678,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,49 +741,49 @@
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="35"/>
+      <c r="H1" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="35"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="21"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>39</v>
-      </c>
       <c r="B2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="10">
         <v>0.9</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="10">
         <v>3</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>37</v>
+      <c r="F2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="I2" s="10">
         <v>0.8</v>
@@ -744,68 +792,72 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="11">
         <v>1.675</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>33</v>
+      <c r="D3" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="E3" s="11">
         <v>3.8</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="28"/>
+      <c r="F3" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="26"/>
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="12">
         <v>2.4750000000000001</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="24"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="33" t="s">
+      <c r="A5" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="32" t="s">
+      <c r="I5" s="30" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="8">
@@ -814,19 +866,27 @@
       <c r="C6" s="13">
         <v>2.2332999999999998</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="23">
         <v>5.9090999999999996</v>
       </c>
       <c r="E6" s="17">
         <v>0.88939999999999997</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="17"/>
+      <c r="F6" s="27">
+        <v>3.1877</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1.52</v>
+      </c>
+      <c r="H6" s="23">
+        <v>1.4877</v>
+      </c>
+      <c r="I6" s="17">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="38" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -835,19 +895,27 @@
       <c r="C7" s="14">
         <v>3.0268000000000002</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>6.7337999999999996</v>
       </c>
       <c r="E7" s="18">
         <v>1.0963000000000001</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="18"/>
+      <c r="F7" s="28">
+        <v>2.6877</v>
+      </c>
+      <c r="G7" s="14">
+        <v>2.52</v>
+      </c>
+      <c r="H7" s="24">
+        <v>5.9877000000000002</v>
+      </c>
+      <c r="I7" s="18">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3">
@@ -856,19 +924,27 @@
       <c r="C8" s="14">
         <v>2.7124000000000001</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>7.4344000000000001</v>
       </c>
       <c r="E8" s="18">
         <v>1.4693000000000001</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="18"/>
+      <c r="F8" s="28">
+        <v>3.6938</v>
+      </c>
+      <c r="G8" s="14">
+        <v>2.52</v>
+      </c>
+      <c r="H8" s="24">
+        <v>3.9937999999999998</v>
+      </c>
+      <c r="I8" s="18">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="38" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
@@ -877,19 +953,27 @@
       <c r="C9" s="14">
         <v>3.3046000000000002</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="24">
         <v>8.0611999999999995</v>
       </c>
       <c r="E9" s="18">
         <v>2.0333999999999999</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="18"/>
+      <c r="F9" s="28">
+        <v>5.4938000000000002</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1.52</v>
+      </c>
+      <c r="H9" s="24">
+        <v>3.4937999999999998</v>
+      </c>
+      <c r="I9" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="3">
@@ -898,19 +982,27 @@
       <c r="C10" s="14">
         <v>3.5518000000000001</v>
       </c>
-      <c r="D10" s="26">
+      <c r="D10" s="24">
         <v>8.5144000000000002</v>
       </c>
       <c r="E10" s="18">
         <v>2.6977000000000002</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="18"/>
+      <c r="F10" s="28">
+        <v>4.9877000000000002</v>
+      </c>
+      <c r="G10" s="14">
+        <v>2.52</v>
+      </c>
+      <c r="H10" s="24">
+        <v>2.9876999999999998</v>
+      </c>
+      <c r="I10" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="38" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="3">
@@ -919,19 +1011,27 @@
       <c r="C11" s="14">
         <v>3.8130000000000002</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="24">
         <v>8.8109000000000002</v>
       </c>
       <c r="E11" s="18">
         <v>3.4727000000000001</v>
       </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="18"/>
+      <c r="F11" s="28">
+        <v>5.9814999999999996</v>
+      </c>
+      <c r="G11" s="14">
+        <v>2.52</v>
+      </c>
+      <c r="H11" s="24">
+        <v>4.4813999999999998</v>
+      </c>
+      <c r="I11" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="38" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="3">
@@ -940,19 +1040,27 @@
       <c r="C12" s="14">
         <v>4.5143000000000004</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="24">
         <v>8.9059000000000008</v>
       </c>
       <c r="E12" s="18">
         <v>4.2782</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="18"/>
+      <c r="F12" s="28">
+        <v>7.8</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1.52</v>
+      </c>
+      <c r="H12" s="24">
+        <v>5.5</v>
+      </c>
+      <c r="I12" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="38" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="3">
@@ -961,19 +1069,27 @@
       <c r="C13" s="14">
         <v>4.4295999999999998</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="24">
         <v>8.7955000000000005</v>
       </c>
       <c r="E13" s="18">
         <v>5.0907</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="18"/>
+      <c r="F13" s="28">
+        <v>7.2938000000000001</v>
+      </c>
+      <c r="G13" s="14">
+        <v>2.52</v>
+      </c>
+      <c r="H13" s="24">
+        <v>6.4938000000000002</v>
+      </c>
+      <c r="I13" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3">
@@ -982,19 +1098,27 @@
       <c r="C14" s="14">
         <v>5.4379999999999997</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="24">
         <v>8.5083000000000002</v>
       </c>
       <c r="E14" s="18">
         <v>5.8545999999999996</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="18"/>
+      <c r="F14" s="28">
+        <v>8.2445000000000004</v>
+      </c>
+      <c r="G14" s="14">
+        <v>2.52</v>
+      </c>
+      <c r="H14" s="24">
+        <v>7.9443999999999999</v>
+      </c>
+      <c r="I14" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="38" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="3">
@@ -1003,19 +1127,27 @@
       <c r="C15" s="14">
         <v>5.0213000000000001</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="24">
         <v>8.0365000000000002</v>
       </c>
       <c r="E15" s="18">
         <v>6.5213000000000001</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="18"/>
+      <c r="F15" s="28">
+        <v>3.1690999999999998</v>
+      </c>
+      <c r="G15" s="14">
+        <v>3.77</v>
+      </c>
+      <c r="H15" s="24">
+        <v>7.4691000000000001</v>
+      </c>
+      <c r="I15" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="3">
@@ -1024,19 +1156,27 @@
       <c r="C16" s="14">
         <v>6.1130000000000004</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="24">
         <v>7.4283000000000001</v>
       </c>
       <c r="E16" s="18">
         <v>7.0754999999999999</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="18"/>
+      <c r="F16" s="28">
+        <v>2.6877</v>
+      </c>
+      <c r="G16" s="14">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="H16" s="24">
+        <v>8.4877000000000002</v>
+      </c>
+      <c r="I16" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="3">
@@ -1045,19 +1185,27 @@
       <c r="C17" s="14">
         <v>5.4101999999999997</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="24">
         <v>6.7035999999999998</v>
       </c>
       <c r="E17" s="18">
         <v>7.4379999999999997</v>
       </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="18"/>
+      <c r="F17" s="28">
+        <v>3.6714000000000002</v>
+      </c>
+      <c r="G17" s="14">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="H17" s="24">
+        <v>9.4713999999999992</v>
+      </c>
+      <c r="I17" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="3">
@@ -1066,19 +1214,27 @@
       <c r="C18" s="14">
         <v>6.3296000000000001</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="24">
         <v>5.9275000000000002</v>
       </c>
       <c r="E18" s="18">
         <v>7.6490999999999998</v>
       </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="18"/>
+      <c r="F18" s="28">
+        <v>7.8060999999999998</v>
+      </c>
+      <c r="G18" s="14">
+        <v>3.77</v>
+      </c>
+      <c r="H18" s="24">
+        <v>8.0061</v>
+      </c>
+      <c r="I18" s="18">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="3">
@@ -1087,19 +1243,27 @@
       <c r="C19" s="14">
         <v>5.5407000000000002</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="24">
         <v>5.0650000000000004</v>
       </c>
       <c r="E19" s="18">
         <v>7.6490999999999998</v>
       </c>
-      <c r="F19" s="30"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="18"/>
+      <c r="F19" s="28">
+        <v>7.2938000000000001</v>
+      </c>
+      <c r="G19" s="14">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="H19" s="24">
+        <v>6.9938000000000002</v>
+      </c>
+      <c r="I19" s="18">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="3">
@@ -1108,19 +1272,27 @@
       <c r="C20" s="14">
         <v>6.1130000000000004</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="24">
         <v>4.2975000000000003</v>
       </c>
       <c r="E20" s="18">
         <v>7.4379999999999997</v>
       </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="18"/>
+      <c r="F20" s="28">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G20" s="14">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="H20" s="24">
+        <v>9</v>
+      </c>
+      <c r="I20" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3">
@@ -1129,19 +1301,27 @@
       <c r="C21" s="14">
         <v>5.4101999999999997</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="24">
         <v>3.5697000000000001</v>
       </c>
       <c r="E21" s="18">
         <v>7.06</v>
       </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="18"/>
+      <c r="F21" s="28">
+        <v>2.6857000000000002</v>
+      </c>
+      <c r="G21" s="14">
+        <v>6.02</v>
+      </c>
+      <c r="H21" s="24">
+        <v>9.9856999999999996</v>
+      </c>
+      <c r="I21" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="38" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="3">
@@ -1150,19 +1330,27 @@
       <c r="C22" s="14">
         <v>5.4379999999999997</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="24">
         <v>2.9573</v>
       </c>
       <c r="E22" s="18">
         <v>6.5213000000000001</v>
       </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="18"/>
+      <c r="F22" s="28">
+        <v>3.7</v>
+      </c>
+      <c r="G22" s="14">
+        <v>6.02</v>
+      </c>
+      <c r="H22" s="24">
+        <v>1</v>
+      </c>
+      <c r="I22" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="38" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="3">
@@ -1171,19 +1359,27 @@
       <c r="C23" s="14">
         <v>5.0213000000000001</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="24">
         <v>2.4969000000000001</v>
       </c>
       <c r="E23" s="18">
         <v>5.8545999999999996</v>
       </c>
-      <c r="F23" s="30"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="18"/>
+      <c r="F23" s="28">
+        <v>2.6938</v>
+      </c>
+      <c r="G23" s="14">
+        <v>7.02</v>
+      </c>
+      <c r="H23" s="24">
+        <v>3.9937999999999998</v>
+      </c>
+      <c r="I23" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="3">
@@ -1192,19 +1388,27 @@
       <c r="C24" s="14">
         <v>4.5143000000000004</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="24">
         <v>2.2019000000000002</v>
       </c>
       <c r="E24" s="18">
         <v>5.0907</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="18"/>
+      <c r="F24" s="28">
+        <v>3.6877</v>
+      </c>
+      <c r="G24" s="14">
+        <v>7.02</v>
+      </c>
+      <c r="H24" s="24">
+        <v>2.4876999999999998</v>
+      </c>
+      <c r="I24" s="18">
+        <v>4.2699999999999996</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="38" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="3">
@@ -1213,19 +1417,27 @@
       <c r="C25" s="14">
         <v>4.4295999999999998</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="24">
         <v>2.0950000000000002</v>
       </c>
       <c r="E25" s="18">
         <v>4.2782</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="18"/>
+      <c r="F25" s="28">
+        <v>5.4794</v>
+      </c>
+      <c r="G25" s="14">
+        <v>6.02</v>
+      </c>
+      <c r="H25" s="24">
+        <v>4.9794</v>
+      </c>
+      <c r="I25" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="38" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="3">
@@ -1234,19 +1446,27 @@
       <c r="C26" s="14">
         <v>3.5518000000000001</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="24">
         <v>2.1959</v>
       </c>
       <c r="E26" s="18">
         <v>3.4727000000000001</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="18"/>
+      <c r="F26" s="28">
+        <v>4.9938000000000002</v>
+      </c>
+      <c r="G26" s="14">
+        <v>7.02</v>
+      </c>
+      <c r="H26" s="24">
+        <v>6.9938000000000002</v>
+      </c>
+      <c r="I26" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="38" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="3">
@@ -1255,19 +1475,27 @@
       <c r="C27" s="14">
         <v>3.8046000000000002</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="24">
         <v>2.4746000000000001</v>
       </c>
       <c r="E27" s="18">
         <v>2.6977000000000002</v>
       </c>
-      <c r="F27" s="30"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="18"/>
+      <c r="F27" s="28">
+        <v>5.9877000000000002</v>
+      </c>
+      <c r="G27" s="14">
+        <v>7.02</v>
+      </c>
+      <c r="H27" s="24">
+        <v>4.9877000000000002</v>
+      </c>
+      <c r="I27" s="18">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="38" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="3">
@@ -1276,19 +1504,27 @@
       <c r="C28" s="14">
         <v>2.7124000000000001</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="24">
         <v>2.9285000000000001</v>
       </c>
       <c r="E28" s="18">
         <v>2.0333999999999999</v>
       </c>
-      <c r="F28" s="30"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="18"/>
+      <c r="F28" s="28">
+        <v>7.3185000000000002</v>
+      </c>
+      <c r="G28" s="14">
+        <v>6.02</v>
+      </c>
+      <c r="H28" s="24">
+        <v>2.0184000000000002</v>
+      </c>
+      <c r="I28" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B29" s="3">
@@ -1297,19 +1533,27 @@
       <c r="C29" s="14">
         <v>3.3046000000000002</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="24">
         <v>3.5438999999999998</v>
       </c>
       <c r="E29" s="18">
         <v>1.4693000000000001</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="18"/>
+      <c r="F29" s="28">
+        <v>8.2876999999999992</v>
+      </c>
+      <c r="G29" s="14">
+        <v>6.02</v>
+      </c>
+      <c r="H29" s="24">
+        <v>2.9876999999999998</v>
+      </c>
+      <c r="I29" s="18">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="38" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="3">
@@ -1318,41 +1562,57 @@
       <c r="C30" s="14">
         <v>2.2332999999999998</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="24">
         <v>4.2803000000000004</v>
       </c>
       <c r="E30" s="18">
         <v>1.0824</v>
       </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="18"/>
+      <c r="F30" s="28">
+        <v>7.2869000000000002</v>
+      </c>
+      <c r="G30" s="14">
+        <v>7.02</v>
+      </c>
+      <c r="H30" s="24">
+        <v>5.9869000000000003</v>
+      </c>
+      <c r="I30" s="18">
+        <v>3.27</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="9">
         <v>5.2045000000000003</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="15">
         <v>3.0268000000000002</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="25">
         <v>5.0795000000000003</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="19">
         <v>0.89300000000000002</v>
       </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="18"/>
+      <c r="F31" s="29">
+        <v>8.2813999999999997</v>
+      </c>
+      <c r="G31" s="15">
+        <v>7.02</v>
+      </c>
+      <c r="H31" s="25">
+        <v>1.9814000000000001</v>
+      </c>
+      <c r="I31" s="19">
+        <v>5.27</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>27</v>
+      <c r="A32" s="39" t="s">
+        <v>42</v>
       </c>
       <c r="B32" s="9">
         <v>5.5</v>
@@ -1360,16 +1620,136 @@
       <c r="C32" s="15">
         <v>4.25</v>
       </c>
-      <c r="D32" s="27">
+      <c r="D32" s="25">
         <v>5.5</v>
       </c>
-      <c r="E32" s="19">
+      <c r="E32" s="45">
         <v>4.25</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="19"/>
+      <c r="F32" s="43">
+        <v>5.5</v>
+      </c>
+      <c r="G32" s="44">
+        <v>4.25</v>
+      </c>
+      <c r="H32" s="45">
+        <v>5.5</v>
+      </c>
+      <c r="I32" s="19">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="40"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="40"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="29"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E35" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="28">
+        <v>3.2</v>
+      </c>
+      <c r="G35" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="28">
+        <v>5.5</v>
+      </c>
+      <c r="G36" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" s="28">
+        <v>7.8</v>
+      </c>
+      <c r="G37" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="28">
+        <v>3.2</v>
+      </c>
+      <c r="G38" s="14">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="28">
+        <v>7.8</v>
+      </c>
+      <c r="G39" s="14">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="28">
+        <v>3.2</v>
+      </c>
+      <c r="G40" s="14">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" s="28">
+        <v>5.5</v>
+      </c>
+      <c r="G41" s="14">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="29">
+        <v>7.8</v>
+      </c>
+      <c r="G42" s="15">
+        <v>6.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>